<commit_message>
Initial commit - stable production version
</commit_message>
<xml_diff>
--- a/fundMetrics_uploads/commodity_trade_CAMS_-_Sikha.xlsx
+++ b/fundMetrics_uploads/commodity_trade_CAMS_-_Sikha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fundMetrics\fundMetrics_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D34D00-4FFD-4B4E-9763-7BB118A82116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB674F7-BAF0-4D6D-8271-EB5EDA320929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="855" windowWidth="21600" windowHeight="11055" xr2:uid="{9A3A6253-3A75-43F4-8991-C2D2AE9F6635}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{9A3A6253-3A75-43F4-8991-C2D2AE9F6635}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -909,14 +909,14 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>